<commit_message>
updated 2 version for budget and Budget Comparison sheet
updated 2 version for budget and Budget Comparison sheet
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\CollegeWork\Agile Project Managment - IT6040\Project-GET IT\IT6040-Agile-Project-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A54B407-B9E3-4D1C-B757-591561D9B51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94FCD72-9B92-47E7-8243-C5539525AA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="v1 (2)" sheetId="2" r:id="rId1"/>
-    <sheet name="v1" sheetId="1" r:id="rId2"/>
+    <sheet name="v1 (3)" sheetId="4" r:id="rId1"/>
+    <sheet name="v1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="v1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="58">
   <si>
     <t>Category</t>
   </si>
@@ -191,13 +192,35 @@
   <si>
     <t xml:space="preserve">office administrative and setup cost </t>
   </si>
+  <si>
+    <t>cost of development of front end design of software , using existign tepmplates for design</t>
+  </si>
+  <si>
+    <t>cost of creating content for tutorial, Only Text Content will be used for website</t>
+  </si>
+  <si>
+    <t>- Text Content</t>
+  </si>
+  <si>
+    <t>No Consultation for Legal complaicnace</t>
+  </si>
+  <si>
+    <t>cost of development of front end design of software , with less expernce Staff</t>
+  </si>
+  <si>
+    <t>cost of creating assists like logo, theme, icon etc,with less expernce Staff</t>
+  </si>
+  <si>
+    <t>cost of creating content for tutorial,with less expernce Staff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -249,7 +272,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +319,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1011,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1245,9 +1274,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
@@ -1264,11 +1290,58 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1548,13 +1621,1422 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16060D28-BA6C-4ED4-9F35-ABFAA3B8932C}">
+  <dimension ref="A1:Q46"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="124" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="35">
+        <f>SUM(D4:I4)</f>
+        <v>31800</v>
+      </c>
+      <c r="D4" s="42">
+        <f t="shared" ref="D4:I4" si="0">SUM(J30:J31)</f>
+        <v>5300</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="I4" s="43">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="125"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="41"/>
+    </row>
+    <row r="6" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="131" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="123" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="35">
+        <f>SUM(D6:I6)</f>
+        <v>4800</v>
+      </c>
+      <c r="D6" s="44">
+        <f>J36</f>
+        <v>800</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" ref="E6:I6" si="1">K36</f>
+        <v>800</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="H6" s="12">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="I6" s="45">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="133" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="126" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="35">
+        <f>SUM(D7:I7)</f>
+        <v>3000</v>
+      </c>
+      <c r="D7" s="46">
+        <f>J38</f>
+        <v>1000</v>
+      </c>
+      <c r="E7" s="15">
+        <f>K38</f>
+        <v>1000</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" ref="F7:I7" si="2">L38</f>
+        <v>1000</v>
+      </c>
+      <c r="G7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="47">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="127"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="41"/>
+    </row>
+    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="132" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="124" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="35">
+        <f>SUM(D9:I9)</f>
+        <v>3000</v>
+      </c>
+      <c r="D9" s="42">
+        <f>SUM(J44:J46)</f>
+        <v>500</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" ref="E9:I9" si="3">SUM(K44:K46)</f>
+        <v>500</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="I9" s="43">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="127"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="41"/>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="124" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="35">
+        <f>SUM(D11:I11)</f>
+        <v>2000</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>500</v>
+      </c>
+      <c r="G11" s="10">
+        <v>500</v>
+      </c>
+      <c r="H11" s="10">
+        <v>500</v>
+      </c>
+      <c r="I11" s="48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="127"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="41"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="124" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="35">
+        <f>SUM(D13:I13)</f>
+        <v>1500</v>
+      </c>
+      <c r="D13" s="42">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>300</v>
+      </c>
+      <c r="F13" s="10">
+        <v>300</v>
+      </c>
+      <c r="G13" s="10">
+        <v>300</v>
+      </c>
+      <c r="H13" s="10">
+        <v>300</v>
+      </c>
+      <c r="I13" s="48">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="127"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="41"/>
+    </row>
+    <row r="15" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="131" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="35">
+        <f>SUM(D15:I15)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="44">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="128"/>
+      <c r="C16" s="35">
+        <f>SUM(D16:I16)</f>
+        <v>3000</v>
+      </c>
+      <c r="D16" s="46">
+        <v>500</v>
+      </c>
+      <c r="E16" s="16">
+        <v>500</v>
+      </c>
+      <c r="F16" s="16">
+        <v>500</v>
+      </c>
+      <c r="G16" s="16">
+        <v>500</v>
+      </c>
+      <c r="H16" s="16">
+        <v>500</v>
+      </c>
+      <c r="I16" s="50">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="127"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="41"/>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="123" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="35">
+        <f>SUM(D18:I18)</f>
+        <v>3600</v>
+      </c>
+      <c r="D18" s="44">
+        <v>600</v>
+      </c>
+      <c r="E18" s="13">
+        <v>600</v>
+      </c>
+      <c r="F18" s="13">
+        <v>600</v>
+      </c>
+      <c r="G18" s="13">
+        <v>600</v>
+      </c>
+      <c r="H18" s="13">
+        <v>600</v>
+      </c>
+      <c r="I18" s="49">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="130" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="129"/>
+      <c r="C19" s="35">
+        <f>SUM(D19:I19)</f>
+        <v>2400</v>
+      </c>
+      <c r="D19" s="51">
+        <v>0</v>
+      </c>
+      <c r="E19" s="18">
+        <v>1200</v>
+      </c>
+      <c r="F19" s="18">
+        <v>0</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0</v>
+      </c>
+      <c r="I19" s="52">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="35">
+        <f>SUM(D20:I20)</f>
+        <v>3000</v>
+      </c>
+      <c r="D20" s="53">
+        <v>500</v>
+      </c>
+      <c r="E20" s="21">
+        <v>500</v>
+      </c>
+      <c r="F20" s="21">
+        <v>500</v>
+      </c>
+      <c r="G20" s="21">
+        <v>500</v>
+      </c>
+      <c r="H20" s="21">
+        <v>500</v>
+      </c>
+      <c r="I20" s="54">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="23">
+        <f>SUM(C4:C20)</f>
+        <v>58100</v>
+      </c>
+      <c r="D21" s="55">
+        <f>SUM(D4:D20)</f>
+        <v>9200</v>
+      </c>
+      <c r="E21" s="56">
+        <f t="shared" ref="E21:I21" si="4">SUM(E4:E20)</f>
+        <v>10700</v>
+      </c>
+      <c r="F21" s="56">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="G21" s="56">
+        <f t="shared" si="4"/>
+        <v>9000</v>
+      </c>
+      <c r="H21" s="56">
+        <f t="shared" si="4"/>
+        <v>9000</v>
+      </c>
+      <c r="I21" s="57">
+        <f t="shared" si="4"/>
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <f>C21-SUM(D21:I21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="122" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="122"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
+      <c r="O26" s="122"/>
+    </row>
+    <row r="27" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="32"/>
+      <c r="B27" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="L27" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="M27" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="N27" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="O27" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="P27" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q27" s="91" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="33"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="83"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="63"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="60"/>
+      <c r="C29" s="58">
+        <f>SUM(C30:C33)</f>
+        <v>390</v>
+      </c>
+      <c r="D29" s="72">
+        <f t="shared" ref="D29:O29" si="5">SUM(D30:D33)</f>
+        <v>65</v>
+      </c>
+      <c r="E29" s="73">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="F29" s="73">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="G29" s="73">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="H29" s="73">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="I29" s="74">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="J29" s="84">
+        <f t="shared" si="5"/>
+        <v>5300</v>
+      </c>
+      <c r="K29" s="85">
+        <f t="shared" si="5"/>
+        <v>5300</v>
+      </c>
+      <c r="L29" s="85">
+        <f t="shared" si="5"/>
+        <v>5300</v>
+      </c>
+      <c r="M29" s="85">
+        <f t="shared" si="5"/>
+        <v>5300</v>
+      </c>
+      <c r="N29" s="85">
+        <f t="shared" si="5"/>
+        <v>5300</v>
+      </c>
+      <c r="O29" s="86">
+        <f t="shared" si="5"/>
+        <v>5300</v>
+      </c>
+      <c r="P29" s="62"/>
+      <c r="Q29" s="63"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="96"/>
+      <c r="B30" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <f>SUM(D30:I30)</f>
+        <v>150</v>
+      </c>
+      <c r="D30" s="69">
+        <v>25</v>
+      </c>
+      <c r="E30" s="70">
+        <v>25</v>
+      </c>
+      <c r="F30" s="70">
+        <v>25</v>
+      </c>
+      <c r="G30" s="70">
+        <v>25</v>
+      </c>
+      <c r="H30" s="70">
+        <v>25</v>
+      </c>
+      <c r="I30" s="71">
+        <v>25</v>
+      </c>
+      <c r="J30" s="81">
+        <f>D30*$P30</f>
+        <v>2500</v>
+      </c>
+      <c r="K30" s="82">
+        <f t="shared" ref="K30:O31" si="6">E30*$P30</f>
+        <v>2500</v>
+      </c>
+      <c r="L30" s="82">
+        <f t="shared" si="6"/>
+        <v>2500</v>
+      </c>
+      <c r="M30" s="82">
+        <f t="shared" si="6"/>
+        <v>2500</v>
+      </c>
+      <c r="N30" s="82">
+        <f t="shared" si="6"/>
+        <v>2500</v>
+      </c>
+      <c r="O30" s="83">
+        <f t="shared" si="6"/>
+        <v>2500</v>
+      </c>
+      <c r="P30" s="62">
+        <v>100</v>
+      </c>
+      <c r="Q30" s="92">
+        <f>SUM(J30:O30)</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="96"/>
+      <c r="B31" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <f>SUM(D31:I31)</f>
+        <v>240</v>
+      </c>
+      <c r="D31" s="69">
+        <v>40</v>
+      </c>
+      <c r="E31" s="70">
+        <v>40</v>
+      </c>
+      <c r="F31" s="70">
+        <v>40</v>
+      </c>
+      <c r="G31" s="70">
+        <v>40</v>
+      </c>
+      <c r="H31" s="70">
+        <v>40</v>
+      </c>
+      <c r="I31" s="71">
+        <v>40</v>
+      </c>
+      <c r="J31" s="81">
+        <f t="shared" ref="J31" si="7">D31*$P31</f>
+        <v>2800</v>
+      </c>
+      <c r="K31" s="82">
+        <f t="shared" si="6"/>
+        <v>2800</v>
+      </c>
+      <c r="L31" s="82">
+        <f t="shared" si="6"/>
+        <v>2800</v>
+      </c>
+      <c r="M31" s="82">
+        <f t="shared" si="6"/>
+        <v>2800</v>
+      </c>
+      <c r="N31" s="82">
+        <f t="shared" si="6"/>
+        <v>2800</v>
+      </c>
+      <c r="O31" s="83">
+        <f t="shared" si="6"/>
+        <v>2800</v>
+      </c>
+      <c r="P31" s="62">
+        <v>70</v>
+      </c>
+      <c r="Q31" s="92">
+        <f>SUM(J31:O31)</f>
+        <v>16800</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="96"/>
+      <c r="B32" s="33"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="83"/>
+      <c r="P32" s="62"/>
+      <c r="Q32" s="92"/>
+    </row>
+    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="96"/>
+      <c r="B33" s="33"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="81"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="83"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="92"/>
+    </row>
+    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="60"/>
+      <c r="C34" s="58">
+        <f t="shared" ref="C34:O34" si="8">SUM(C36:C37)</f>
+        <v>60</v>
+      </c>
+      <c r="D34" s="72">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="E34" s="73">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="F34" s="73">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="G34" s="73">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="H34" s="73">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="I34" s="74">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="J34" s="84">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="K34" s="85">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="L34" s="85">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="M34" s="85">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="N34" s="85">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="O34" s="86">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
+      <c r="P34" s="62"/>
+      <c r="Q34" s="92"/>
+    </row>
+    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="33"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="82"/>
+      <c r="N35" s="82"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="62"/>
+      <c r="Q35" s="92"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="96"/>
+      <c r="B36" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <f>SUM(D36:I36)</f>
+        <v>60</v>
+      </c>
+      <c r="D36" s="69">
+        <v>10</v>
+      </c>
+      <c r="E36" s="70">
+        <v>10</v>
+      </c>
+      <c r="F36" s="70">
+        <v>10</v>
+      </c>
+      <c r="G36" s="70">
+        <v>10</v>
+      </c>
+      <c r="H36" s="70">
+        <v>10</v>
+      </c>
+      <c r="I36" s="71">
+        <v>10</v>
+      </c>
+      <c r="J36" s="81">
+        <f>D36*$P36</f>
+        <v>800</v>
+      </c>
+      <c r="K36" s="82">
+        <f t="shared" ref="K36:O36" si="9">E36*$P36</f>
+        <v>800</v>
+      </c>
+      <c r="L36" s="82">
+        <f t="shared" si="9"/>
+        <v>800</v>
+      </c>
+      <c r="M36" s="82">
+        <f t="shared" si="9"/>
+        <v>800</v>
+      </c>
+      <c r="N36" s="82">
+        <f t="shared" si="9"/>
+        <v>800</v>
+      </c>
+      <c r="O36" s="83">
+        <f t="shared" si="9"/>
+        <v>800</v>
+      </c>
+      <c r="P36" s="62">
+        <v>80</v>
+      </c>
+      <c r="Q36" s="92">
+        <f>SUM(J36:O36)</f>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="96"/>
+      <c r="B37" s="33"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="82"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="83"/>
+      <c r="P37" s="62"/>
+      <c r="Q37" s="92"/>
+    </row>
+    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="60"/>
+      <c r="C38" s="58">
+        <f>SUM(C39:C41)</f>
+        <v>60</v>
+      </c>
+      <c r="D38" s="72">
+        <f t="shared" ref="D38:O38" si="10">SUM(D39:D41)</f>
+        <v>20</v>
+      </c>
+      <c r="E38" s="73">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="F38" s="73">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="G38" s="73">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="73">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="74">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="84">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="K38" s="85">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="L38" s="85">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="M38" s="85">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="85">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O38" s="86">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="92"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="96"/>
+      <c r="B39" s="32"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="81"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="82"/>
+      <c r="M39" s="82"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="83"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="92"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="96"/>
+      <c r="B40" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40">
+        <f>SUM(D40:I40)</f>
+        <v>60</v>
+      </c>
+      <c r="D40" s="69">
+        <v>20</v>
+      </c>
+      <c r="E40" s="70">
+        <v>20</v>
+      </c>
+      <c r="F40" s="70">
+        <v>20</v>
+      </c>
+      <c r="G40" s="70">
+        <v>0</v>
+      </c>
+      <c r="H40" s="70">
+        <v>0</v>
+      </c>
+      <c r="I40" s="71">
+        <v>0</v>
+      </c>
+      <c r="J40" s="81">
+        <f>D40*$P40</f>
+        <v>1000</v>
+      </c>
+      <c r="K40" s="82">
+        <f t="shared" ref="K40:O40" si="11">E40*$P40</f>
+        <v>1000</v>
+      </c>
+      <c r="L40" s="82">
+        <f t="shared" si="11"/>
+        <v>1000</v>
+      </c>
+      <c r="M40" s="82">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="82">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="83">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="62">
+        <v>50</v>
+      </c>
+      <c r="Q40" s="92">
+        <f>SUM(J40:O40)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="96"/>
+      <c r="B41" s="34"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="82"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="82"/>
+      <c r="N41" s="82"/>
+      <c r="O41" s="83"/>
+      <c r="P41" s="62"/>
+      <c r="Q41" s="92"/>
+    </row>
+    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="60"/>
+      <c r="C42" s="58">
+        <f t="shared" ref="C42:O42" si="12">SUM(C44:C46)</f>
+        <v>180</v>
+      </c>
+      <c r="D42" s="72">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="E42" s="73">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="F42" s="73">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="G42" s="73">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="H42" s="73">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="I42" s="74">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="J42" s="84">
+        <f t="shared" si="12"/>
+        <v>500</v>
+      </c>
+      <c r="K42" s="85">
+        <f t="shared" si="12"/>
+        <v>500</v>
+      </c>
+      <c r="L42" s="85">
+        <f t="shared" si="12"/>
+        <v>500</v>
+      </c>
+      <c r="M42" s="85">
+        <f t="shared" si="12"/>
+        <v>500</v>
+      </c>
+      <c r="N42" s="85">
+        <f t="shared" si="12"/>
+        <v>500</v>
+      </c>
+      <c r="O42" s="86">
+        <f t="shared" si="12"/>
+        <v>500</v>
+      </c>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="92"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="33"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="81"/>
+      <c r="K43" s="82"/>
+      <c r="L43" s="82"/>
+      <c r="M43" s="82"/>
+      <c r="N43" s="82"/>
+      <c r="O43" s="83"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="92"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="96"/>
+      <c r="B44" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44">
+        <f>SUM(D44:I44)</f>
+        <v>60</v>
+      </c>
+      <c r="D44" s="69">
+        <v>10</v>
+      </c>
+      <c r="E44" s="70">
+        <v>10</v>
+      </c>
+      <c r="F44" s="70">
+        <v>10</v>
+      </c>
+      <c r="G44" s="70">
+        <v>10</v>
+      </c>
+      <c r="H44" s="70">
+        <v>10</v>
+      </c>
+      <c r="I44" s="71">
+        <v>10</v>
+      </c>
+      <c r="J44" s="81">
+        <f t="shared" ref="J44:O46" si="13">D44*$P44</f>
+        <v>500</v>
+      </c>
+      <c r="K44" s="82">
+        <f t="shared" si="13"/>
+        <v>500</v>
+      </c>
+      <c r="L44" s="82">
+        <f t="shared" si="13"/>
+        <v>500</v>
+      </c>
+      <c r="M44" s="82">
+        <f t="shared" si="13"/>
+        <v>500</v>
+      </c>
+      <c r="N44" s="82">
+        <f t="shared" si="13"/>
+        <v>500</v>
+      </c>
+      <c r="O44" s="83">
+        <f t="shared" si="13"/>
+        <v>500</v>
+      </c>
+      <c r="P44" s="62">
+        <v>50</v>
+      </c>
+      <c r="Q44" s="92">
+        <f>SUM(J44:O44)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="33"/>
+      <c r="B45" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <f>SUM(D45:I45)</f>
+        <v>60</v>
+      </c>
+      <c r="D45" s="69">
+        <v>10</v>
+      </c>
+      <c r="E45" s="70">
+        <v>10</v>
+      </c>
+      <c r="F45" s="70">
+        <v>10</v>
+      </c>
+      <c r="G45" s="70">
+        <v>10</v>
+      </c>
+      <c r="H45" s="70">
+        <v>10</v>
+      </c>
+      <c r="I45" s="71">
+        <v>10</v>
+      </c>
+      <c r="J45" s="81">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="82">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="82">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="82">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="N45" s="82">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O45" s="83">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P45" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="92">
+        <f>SUM(J45:O45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="34"/>
+      <c r="B46" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="65">
+        <f>SUM(D46:I46)</f>
+        <v>60</v>
+      </c>
+      <c r="D46" s="75">
+        <v>10</v>
+      </c>
+      <c r="E46" s="76">
+        <v>10</v>
+      </c>
+      <c r="F46" s="76">
+        <v>10</v>
+      </c>
+      <c r="G46" s="76">
+        <v>10</v>
+      </c>
+      <c r="H46" s="76">
+        <v>10</v>
+      </c>
+      <c r="I46" s="77">
+        <v>10</v>
+      </c>
+      <c r="J46" s="87">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K46" s="88">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="88">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="88">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="N46" s="88">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O46" s="89">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="64">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="61">
+        <f>SUM(J46:O46)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="J26:O26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDC5371-1000-4D78-AB43-43C781A04A11}">
-  <dimension ref="A1:AB52"/>
+  <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A23" sqref="A23"/>
-      <selection pane="topRight" activeCell="E48" sqref="E48"/>
+      <selection pane="topRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,12 +3146,12 @@
       <c r="H5" s="6"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:9" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:9" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="131" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C6" s="35">
         <f>SUM(D6:I6)</f>
@@ -1700,12 +3182,12 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A7" s="133" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C7" s="35">
         <f>SUM(D7:I7)</f>
@@ -1750,11 +3232,11 @@
       <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="134" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C9" s="35">
         <f>SUM(D9:I9)</f>
@@ -1885,7 +3367,7 @@
       <c r="I14" s="41"/>
     </row>
     <row r="15" spans="1:9" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="135" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="26" t="s">
@@ -1986,7 +3468,7 @@
       </c>
     </row>
     <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="136" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="30"/>
@@ -2082,22 +3564,22 @@
       </c>
     </row>
     <row r="26" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="100" t="s">
+      <c r="D26" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="100"/>
-      <c r="I26" s="100"/>
-      <c r="J26" s="100" t="s">
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="100"/>
-      <c r="L26" s="100"/>
-      <c r="M26" s="100"/>
-      <c r="N26" s="100"/>
-      <c r="O26" s="100"/>
+      <c r="K26" s="122"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
+      <c r="O26" s="122"/>
     </row>
     <row r="27" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="32"/>
@@ -2149,22 +3631,22 @@
       <c r="Q27" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="W27" s="101" t="s">
+      <c r="W27" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="X27" s="115" t="s">
+      <c r="X27" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="Y27" s="109" t="s">
+      <c r="Y27" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="Z27" s="110" t="s">
+      <c r="Z27" s="109" t="s">
         <v>47</v>
       </c>
-      <c r="AA27" s="103" t="s">
+      <c r="AA27" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="AB27" s="104" t="s">
+      <c r="AB27" s="103" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2188,11 +3670,10 @@
       <c r="P28" s="62"/>
       <c r="Q28" s="63"/>
       <c r="W28" s="62"/>
-      <c r="X28" s="116"/>
-      <c r="Y28" s="111"/>
-      <c r="Z28" s="112"/>
-      <c r="AA28" s="105"/>
-      <c r="AB28" s="106"/>
+      <c r="Y28" s="110"/>
+      <c r="Z28" s="111"/>
+      <c r="AA28" s="104"/>
+      <c r="AB28" s="105"/>
     </row>
     <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="95" t="s">
@@ -2254,11 +3735,10 @@
       <c r="P29" s="62"/>
       <c r="Q29" s="63"/>
       <c r="W29" s="62"/>
-      <c r="X29" s="116"/>
-      <c r="Y29" s="111"/>
-      <c r="Z29" s="112"/>
-      <c r="AA29" s="105"/>
-      <c r="AB29" s="106"/>
+      <c r="Y29" s="110"/>
+      <c r="Z29" s="111"/>
+      <c r="AA29" s="104"/>
+      <c r="AB29" s="105"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="96"/>
@@ -2321,19 +3801,19 @@
       <c r="W30" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="X30" s="116">
+      <c r="X30">
         <v>150</v>
       </c>
-      <c r="Y30" s="111">
+      <c r="Y30" s="110">
         <v>60</v>
       </c>
-      <c r="Z30" s="112">
+      <c r="Z30" s="111">
         <v>9000</v>
       </c>
-      <c r="AA30" s="105">
+      <c r="AA30" s="104">
         <v>100</v>
       </c>
-      <c r="AB30" s="106">
+      <c r="AB30" s="105">
         <v>15000</v>
       </c>
     </row>
@@ -2398,19 +3878,19 @@
       <c r="W31" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="X31" s="116">
+      <c r="X31">
         <v>240</v>
       </c>
-      <c r="Y31" s="111">
+      <c r="Y31" s="110">
         <v>40</v>
       </c>
-      <c r="Z31" s="112">
+      <c r="Z31" s="111">
         <v>9600</v>
       </c>
-      <c r="AA31" s="105">
+      <c r="AA31" s="104">
         <v>70</v>
       </c>
-      <c r="AB31" s="106">
+      <c r="AB31" s="105">
         <v>16800</v>
       </c>
     </row>
@@ -2432,11 +3912,10 @@
       <c r="P32" s="62"/>
       <c r="Q32" s="92"/>
       <c r="W32" s="62"/>
-      <c r="X32" s="116"/>
-      <c r="Y32" s="111"/>
-      <c r="Z32" s="112"/>
-      <c r="AA32" s="105"/>
-      <c r="AB32" s="106"/>
+      <c r="Y32" s="110"/>
+      <c r="Z32" s="111"/>
+      <c r="AA32" s="104"/>
+      <c r="AB32" s="105"/>
     </row>
     <row r="33" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="96"/>
@@ -2456,11 +3935,10 @@
       <c r="P33" s="93"/>
       <c r="Q33" s="92"/>
       <c r="W33" s="62"/>
-      <c r="X33" s="116"/>
-      <c r="Y33" s="111"/>
-      <c r="Z33" s="112"/>
-      <c r="AA33" s="105"/>
-      <c r="AB33" s="106"/>
+      <c r="Y33" s="110"/>
+      <c r="Z33" s="111"/>
+      <c r="AA33" s="104"/>
+      <c r="AB33" s="105"/>
     </row>
     <row r="34" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="97" t="s">
@@ -2522,11 +4000,10 @@
       <c r="P34" s="62"/>
       <c r="Q34" s="92"/>
       <c r="W34" s="62"/>
-      <c r="X34" s="116"/>
-      <c r="Y34" s="111"/>
-      <c r="Z34" s="112"/>
-      <c r="AA34" s="105"/>
-      <c r="AB34" s="106"/>
+      <c r="Y34" s="110"/>
+      <c r="Z34" s="111"/>
+      <c r="AA34" s="104"/>
+      <c r="AB34" s="105"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="98" t="s">
@@ -2548,11 +4025,10 @@
       <c r="P35" s="62"/>
       <c r="Q35" s="92"/>
       <c r="W35" s="62"/>
-      <c r="X35" s="116"/>
-      <c r="Y35" s="111"/>
-      <c r="Z35" s="112"/>
-      <c r="AA35" s="105"/>
-      <c r="AB35" s="106"/>
+      <c r="Y35" s="110"/>
+      <c r="Z35" s="111"/>
+      <c r="AA35" s="104"/>
+      <c r="AB35" s="105"/>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="96"/>
@@ -2615,19 +4091,19 @@
       <c r="W36" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="X36" s="116">
+      <c r="X36">
         <v>150</v>
       </c>
-      <c r="Y36" s="111">
+      <c r="Y36" s="110">
         <v>50</v>
       </c>
-      <c r="Z36" s="112">
+      <c r="Z36" s="111">
         <v>7500</v>
       </c>
-      <c r="AA36" s="105">
+      <c r="AA36" s="104">
         <v>80</v>
       </c>
-      <c r="AB36" s="106">
+      <c r="AB36" s="105">
         <v>12000</v>
       </c>
     </row>
@@ -2649,11 +4125,10 @@
       <c r="P37" s="62"/>
       <c r="Q37" s="92"/>
       <c r="W37" s="62"/>
-      <c r="X37" s="116"/>
-      <c r="Y37" s="111"/>
-      <c r="Z37" s="112"/>
-      <c r="AA37" s="105"/>
-      <c r="AB37" s="106"/>
+      <c r="Y37" s="110"/>
+      <c r="Z37" s="111"/>
+      <c r="AA37" s="104"/>
+      <c r="AB37" s="105"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="95" t="s">
@@ -2715,11 +4190,10 @@
       <c r="P38" s="62"/>
       <c r="Q38" s="92"/>
       <c r="W38" s="62"/>
-      <c r="X38" s="116"/>
-      <c r="Y38" s="111"/>
-      <c r="Z38" s="112"/>
-      <c r="AA38" s="105"/>
-      <c r="AB38" s="106"/>
+      <c r="Y38" s="110"/>
+      <c r="Z38" s="111"/>
+      <c r="AA38" s="104"/>
+      <c r="AB38" s="105"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="96"/>
@@ -2739,11 +4213,10 @@
       <c r="P39" s="62"/>
       <c r="Q39" s="92"/>
       <c r="W39" s="62"/>
-      <c r="X39" s="116"/>
-      <c r="Y39" s="111"/>
-      <c r="Z39" s="112"/>
-      <c r="AA39" s="105"/>
-      <c r="AB39" s="106"/>
+      <c r="Y39" s="110"/>
+      <c r="Z39" s="111"/>
+      <c r="AA39" s="104"/>
+      <c r="AB39" s="105"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="96"/>
@@ -2806,19 +4279,19 @@
       <c r="W40" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="X40" s="116">
+      <c r="X40">
         <v>60</v>
       </c>
-      <c r="Y40" s="111">
+      <c r="Y40" s="110">
         <v>30</v>
       </c>
-      <c r="Z40" s="112">
+      <c r="Z40" s="111">
         <v>1800</v>
       </c>
-      <c r="AA40" s="105">
+      <c r="AA40" s="104">
         <v>50</v>
       </c>
-      <c r="AB40" s="106">
+      <c r="AB40" s="105">
         <v>3000</v>
       </c>
     </row>
@@ -2840,11 +4313,10 @@
       <c r="P41" s="62"/>
       <c r="Q41" s="92"/>
       <c r="W41" s="62"/>
-      <c r="X41" s="116"/>
-      <c r="Y41" s="111"/>
-      <c r="Z41" s="112"/>
-      <c r="AA41" s="105"/>
-      <c r="AB41" s="106"/>
+      <c r="Y41" s="110"/>
+      <c r="Z41" s="111"/>
+      <c r="AA41" s="104"/>
+      <c r="AB41" s="105"/>
     </row>
     <row r="42" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="97" t="s">
@@ -2906,11 +4378,10 @@
       <c r="P42" s="62"/>
       <c r="Q42" s="92"/>
       <c r="W42" s="62"/>
-      <c r="X42" s="116"/>
-      <c r="Y42" s="111"/>
-      <c r="Z42" s="112"/>
-      <c r="AA42" s="105"/>
-      <c r="AB42" s="106"/>
+      <c r="Y42" s="110"/>
+      <c r="Z42" s="111"/>
+      <c r="AA42" s="104"/>
+      <c r="AB42" s="105"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="99" t="s">
@@ -2932,11 +4403,10 @@
       <c r="P43" s="62"/>
       <c r="Q43" s="92"/>
       <c r="W43" s="62"/>
-      <c r="X43" s="116"/>
-      <c r="Y43" s="111"/>
-      <c r="Z43" s="112"/>
-      <c r="AA43" s="105"/>
-      <c r="AB43" s="106"/>
+      <c r="Y43" s="110"/>
+      <c r="Z43" s="111"/>
+      <c r="AA43" s="104"/>
+      <c r="AB43" s="105"/>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="96"/>
@@ -2999,19 +4469,19 @@
       <c r="W44" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="X44" s="116">
+      <c r="X44">
         <v>60</v>
       </c>
-      <c r="Y44" s="111">
+      <c r="Y44" s="110">
         <v>30</v>
       </c>
-      <c r="Z44" s="112">
+      <c r="Z44" s="111">
         <v>1800</v>
       </c>
-      <c r="AA44" s="105">
+      <c r="AA44" s="104">
         <v>50</v>
       </c>
-      <c r="AB44" s="106">
+      <c r="AB44" s="105">
         <v>3000</v>
       </c>
     </row>
@@ -3076,19 +4546,19 @@
       <c r="W45" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="X45" s="116">
+      <c r="X45">
         <v>60</v>
       </c>
-      <c r="Y45" s="111">
+      <c r="Y45" s="110">
         <v>30</v>
       </c>
-      <c r="Z45" s="112">
+      <c r="Z45" s="111">
         <v>1800</v>
       </c>
-      <c r="AA45" s="105">
+      <c r="AA45" s="104">
         <v>50</v>
       </c>
-      <c r="AB45" s="106">
+      <c r="AB45" s="105">
         <v>3000</v>
       </c>
     </row>
@@ -3156,82 +4626,100 @@
       <c r="X46" s="65">
         <v>60</v>
       </c>
-      <c r="Y46" s="113">
+      <c r="Y46" s="112">
         <v>30</v>
       </c>
-      <c r="Z46" s="114">
+      <c r="Z46" s="113">
         <v>1800</v>
       </c>
-      <c r="AA46" s="107">
+      <c r="AA46" s="106">
         <v>50</v>
       </c>
-      <c r="AB46" s="108">
+      <c r="AB46" s="107">
         <v>3000</v>
       </c>
     </row>
     <row r="47" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="W48" s="101" t="s">
+      <c r="W48" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="X48" s="115"/>
-      <c r="Y48" s="115"/>
-      <c r="Z48" s="115">
+      <c r="X48" s="119">
+        <v>0.85</v>
+      </c>
+      <c r="Y48" s="120">
+        <f>(Z48/Z52)*100</f>
+        <v>65.294117647058826</v>
+      </c>
+      <c r="Z48" s="114">
         <f>SUM(Z28:Z46)</f>
         <v>33300</v>
       </c>
-      <c r="AA48" s="115"/>
-      <c r="AB48" s="102">
+      <c r="AA48" s="120">
+        <f>(AB48/AB52)*100</f>
+        <v>75.91836734693878</v>
+      </c>
+      <c r="AB48" s="101">
         <f>SUM(AB28:AB46)</f>
         <v>55800</v>
       </c>
     </row>
     <row r="49" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W49" s="62"/>
-      <c r="X49" s="116"/>
-      <c r="Y49" s="116"/>
-      <c r="Z49" s="116"/>
-      <c r="AA49" s="116"/>
       <c r="AB49" s="63"/>
     </row>
     <row r="50" spans="23:28" x14ac:dyDescent="0.25">
       <c r="W50" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="X50" s="116"/>
-      <c r="Y50" s="116"/>
-      <c r="Z50" s="117">
+      <c r="X50" s="121">
+        <v>0.15</v>
+      </c>
+      <c r="Y50" s="118">
+        <f>(Z50/Z52)*100</f>
+        <v>34.705882352941174</v>
+      </c>
+      <c r="Z50" s="8">
         <f>+AB50</f>
         <v>17700</v>
       </c>
-      <c r="AA50" s="116"/>
-      <c r="AB50" s="118">
+      <c r="AA50" s="118">
+        <f>(AB50/AB52)*100</f>
+        <v>24.081632653061224</v>
+      </c>
+      <c r="AB50" s="115">
         <f>'v1'!C21-AB48</f>
         <v>17700</v>
       </c>
     </row>
     <row r="51" spans="23:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="W51" s="62"/>
-      <c r="X51" s="116"/>
-      <c r="Y51" s="116"/>
-      <c r="Z51" s="116"/>
-      <c r="AA51" s="116"/>
       <c r="AB51" s="63"/>
     </row>
     <row r="52" spans="23:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="W52" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="X52" s="119"/>
-      <c r="Y52" s="119"/>
-      <c r="Z52" s="120">
+      <c r="X52" s="116"/>
+      <c r="Y52" s="116"/>
+      <c r="Z52" s="117">
         <f>SUM(Z48:Z50)</f>
         <v>51000</v>
       </c>
-      <c r="AA52" s="120"/>
+      <c r="AA52" s="117"/>
       <c r="AB52" s="59">
         <f>SUM(AB48:AB50)</f>
         <v>73500</v>
+      </c>
+    </row>
+    <row r="55" spans="23:28" x14ac:dyDescent="0.25">
+      <c r="Z55" s="118">
+        <f>(Z50/Z52)*100</f>
+        <v>34.705882352941174</v>
+      </c>
+      <c r="AB55" s="118">
+        <f>(AB50/AB52)*100</f>
+        <v>24.081632653061224</v>
       </c>
     </row>
   </sheetData>
@@ -3244,12 +4732,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27:Q46"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3772,22 +5260,22 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="100" t="s">
+      <c r="D26" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="100"/>
-      <c r="I26" s="100"/>
-      <c r="J26" s="100" t="s">
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="100"/>
-      <c r="L26" s="100"/>
-      <c r="M26" s="100"/>
-      <c r="N26" s="100"/>
-      <c r="O26" s="100"/>
+      <c r="K26" s="122"/>
+      <c r="L26" s="122"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
+      <c r="O26" s="122"/>
     </row>
     <row r="27" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="32"/>

</xml_diff>

<commit_message>
Updated Increased Budget -100k
updated increased budget -100k
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\CollegeWork\Agile Project Managment - IT6040\Project-GET IT\IT6040-Agile-Project-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94FCD72-9B92-47E7-8243-C5539525AA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9B1839-D49B-4291-91FA-8CD66D11178A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="v1 (3)" sheetId="4" r:id="rId1"/>
-    <sheet name="v1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="v1" sheetId="1" r:id="rId3"/>
+    <sheet name="v1 (4)" sheetId="5" r:id="rId1"/>
+    <sheet name="v1 (3)" sheetId="4" r:id="rId2"/>
+    <sheet name="v1 (2)" sheetId="2" r:id="rId3"/>
+    <sheet name="v1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="64">
   <si>
     <t>Category</t>
   </si>
@@ -212,6 +213,24 @@
   </si>
   <si>
     <t>cost of creating content for tutorial,with less expernce Staff</t>
+  </si>
+  <si>
+    <t>Security Consultant</t>
+  </si>
+  <si>
+    <t>Improved security for data</t>
+  </si>
+  <si>
+    <t>improved user experience based on research findings</t>
+  </si>
+  <si>
+    <t>- Data Security</t>
+  </si>
+  <si>
+    <t>Research and Development</t>
+  </si>
+  <si>
+    <t>-R&amp;D for Ui and UX design and usability</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1059,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1297,49 +1316,70 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1621,25 +1661,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16060D28-BA6C-4ED4-9F35-ABFAA3B8932C}">
-  <dimension ref="A1:Q46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404F1782-9262-4FF0-9DE7-1C9890B559EA}">
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I21"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="15" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:14" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1668,7 +1708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1681,11 +1721,11 @@
       <c r="H3" s="6"/>
       <c r="I3" s="41"/>
     </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="24" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="35">
@@ -1693,7 +1733,7 @@
         <v>31800</v>
       </c>
       <c r="D4" s="42">
-        <f t="shared" ref="D4:I4" si="0">SUM(J30:J31)</f>
+        <f t="shared" ref="D4:I4" si="0">SUM(J34:J35)</f>
         <v>5300</v>
       </c>
       <c r="E4" s="9">
@@ -1717,11 +1757,11 @@
         <v>5300</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="125"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="36"/>
       <c r="D5" s="40"/>
       <c r="E5" s="6"/>
@@ -1730,47 +1770,47 @@
       <c r="H5" s="6"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="131" t="s">
+    <row r="6" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="123" t="s">
-        <v>51</v>
+      <c r="B6" s="26" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="35">
         <f>SUM(D6:I6)</f>
-        <v>4800</v>
+        <v>12000</v>
       </c>
       <c r="D6" s="44">
-        <f>J36</f>
-        <v>800</v>
+        <f>J40</f>
+        <v>2000</v>
       </c>
       <c r="E6" s="12">
-        <f t="shared" ref="E6:I6" si="1">K36</f>
-        <v>800</v>
+        <f t="shared" ref="E6:I6" si="1">K40</f>
+        <v>2000</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="G6" s="12">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="I6" s="45">
         <f t="shared" si="1"/>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="133" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="35">
@@ -1778,15 +1818,15 @@
         <v>3000</v>
       </c>
       <c r="D7" s="46">
-        <f>J38</f>
+        <f>J42</f>
         <v>1000</v>
       </c>
       <c r="E7" s="15">
-        <f>K38</f>
+        <f>K42</f>
         <v>1000</v>
       </c>
       <c r="F7" s="15">
-        <f t="shared" ref="F7:I7" si="2">L38</f>
+        <f t="shared" ref="F7:I7" si="2">L42</f>
         <v>1000</v>
       </c>
       <c r="G7" s="15">
@@ -1802,11 +1842,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="127"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="36"/>
       <c r="D8" s="40"/>
       <c r="E8" s="6"/>
@@ -1815,47 +1855,47 @@
       <c r="H8" s="6"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="132" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="124" t="s">
-        <v>52</v>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="35">
         <f>SUM(D9:I9)</f>
-        <v>3000</v>
+        <v>9000</v>
       </c>
       <c r="D9" s="42">
-        <f>SUM(J44:J46)</f>
-        <v>500</v>
+        <f>SUM(J48:J50)</f>
+        <v>1500</v>
       </c>
       <c r="E9" s="9">
-        <f t="shared" ref="E9:I9" si="3">SUM(K44:K46)</f>
-        <v>500</v>
+        <f t="shared" ref="E9:I9" si="3">SUM(K48:K50)</f>
+        <v>1500</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="I9" s="43">
         <f t="shared" si="3"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="127"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="36"/>
       <c r="D10" s="40"/>
       <c r="E10" s="6"/>
@@ -1864,11 +1904,11 @@
       <c r="H10" s="6"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="124" t="s">
+      <c r="B11" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="35">
@@ -1894,11 +1934,1513 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="137"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="140"/>
+      <c r="I12" s="141"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="142" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="35">
+        <f>SUM(D13:I13)</f>
+        <v>5000</v>
+      </c>
+      <c r="D13" s="42">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>5000</v>
+      </c>
+      <c r="I13" s="48">
+        <v>0</v>
+      </c>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="41"/>
+    </row>
+    <row r="15" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="143" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="35">
+        <f>SUM(D15:I15)</f>
+        <v>5000</v>
+      </c>
+      <c r="D15" s="42">
+        <f>SUM(J54:J56)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>5000</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" ref="F15" si="4">SUM(L54:L56)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" ref="G15" si="5">SUM(M54:M56)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" ref="H15" si="6">SUM(N54:N56)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="43">
+        <f t="shared" ref="I15" si="7">SUM(O54:O56)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="41"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="35">
+        <f>SUM(D17:I17)</f>
+        <v>10500</v>
+      </c>
+      <c r="D17" s="42">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>2100</v>
+      </c>
+      <c r="F17" s="10">
+        <v>2100</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2100</v>
+      </c>
+      <c r="H17" s="10">
+        <v>2100</v>
+      </c>
+      <c r="I17" s="48">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="41"/>
+    </row>
+    <row r="19" spans="1:17" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="35">
+        <f>SUM(D19:I19)</f>
+        <v>1000</v>
+      </c>
+      <c r="D19" s="44">
+        <v>500</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0</v>
+      </c>
+      <c r="F19" s="13">
+        <v>0</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0</v>
+      </c>
+      <c r="H19" s="13">
+        <v>500</v>
+      </c>
+      <c r="I19" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="35">
+        <f>SUM(D20:I20)</f>
+        <v>10000</v>
+      </c>
+      <c r="D20" s="46">
+        <v>500</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1900</v>
+      </c>
+      <c r="F20" s="16">
+        <v>1900</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1900</v>
+      </c>
+      <c r="H20" s="16">
+        <v>1900</v>
+      </c>
+      <c r="I20" s="50">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="35">
+        <f>SUM(D22:I22)</f>
+        <v>3600</v>
+      </c>
+      <c r="D22" s="44">
+        <v>600</v>
+      </c>
+      <c r="E22" s="13">
+        <v>600</v>
+      </c>
+      <c r="F22" s="13">
+        <v>600</v>
+      </c>
+      <c r="G22" s="13">
+        <v>600</v>
+      </c>
+      <c r="H22" s="13">
+        <v>600</v>
+      </c>
+      <c r="I22" s="49">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="35">
+        <f>SUM(D23:I23)</f>
+        <v>4100</v>
+      </c>
+      <c r="D23" s="51">
+        <v>0</v>
+      </c>
+      <c r="E23" s="18">
+        <v>1200</v>
+      </c>
+      <c r="F23" s="18">
+        <v>0</v>
+      </c>
+      <c r="G23" s="18">
+        <v>1700</v>
+      </c>
+      <c r="H23" s="18">
+        <v>0</v>
+      </c>
+      <c r="I23" s="52">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="35">
+        <f>SUM(D24:I24)</f>
+        <v>3000</v>
+      </c>
+      <c r="D24" s="53">
+        <v>500</v>
+      </c>
+      <c r="E24" s="21">
+        <v>500</v>
+      </c>
+      <c r="F24" s="21">
+        <v>500</v>
+      </c>
+      <c r="G24" s="21">
+        <v>500</v>
+      </c>
+      <c r="H24" s="21">
+        <v>500</v>
+      </c>
+      <c r="I24" s="54">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="23">
+        <f>SUM(C4:C24)</f>
+        <v>100000</v>
+      </c>
+      <c r="D25" s="55">
+        <f>SUM(D4:D24)</f>
+        <v>11900</v>
+      </c>
+      <c r="E25" s="56">
+        <f>SUM(E4:E24)</f>
+        <v>21100</v>
+      </c>
+      <c r="F25" s="56">
+        <f>SUM(F4:F24)</f>
+        <v>15400</v>
+      </c>
+      <c r="G25" s="56">
+        <f>SUM(G4:G24)</f>
+        <v>16100</v>
+      </c>
+      <c r="H25" s="56">
+        <f>SUM(H4:H24)</f>
+        <v>19900</v>
+      </c>
+      <c r="I25" s="57">
+        <f>SUM(I4:I24)</f>
+        <v>15600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <f>C25-SUM(D25:I25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="136" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="136"/>
+      <c r="H30" s="136"/>
+      <c r="I30" s="136"/>
+      <c r="J30" s="136" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="136"/>
+      <c r="L30" s="136"/>
+      <c r="M30" s="136"/>
+      <c r="N30" s="136"/>
+      <c r="O30" s="136"/>
+    </row>
+    <row r="31" spans="1:17" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="32"/>
+      <c r="B31" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="K31" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="L31" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="M31" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="O31" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="P31" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q31" s="91" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="83"/>
+      <c r="P32" s="62"/>
+      <c r="Q32" s="63"/>
+    </row>
+    <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="60"/>
+      <c r="C33" s="58">
+        <f>SUM(C34:C37)</f>
+        <v>390</v>
+      </c>
+      <c r="D33" s="72">
+        <f t="shared" ref="D33:O33" si="8">SUM(D34:D37)</f>
+        <v>65</v>
+      </c>
+      <c r="E33" s="73">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="F33" s="73">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="G33" s="73">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="H33" s="73">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="I33" s="74">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="J33" s="84">
+        <f t="shared" si="8"/>
+        <v>5300</v>
+      </c>
+      <c r="K33" s="85">
+        <f t="shared" si="8"/>
+        <v>5300</v>
+      </c>
+      <c r="L33" s="85">
+        <f t="shared" si="8"/>
+        <v>5300</v>
+      </c>
+      <c r="M33" s="85">
+        <f t="shared" si="8"/>
+        <v>5300</v>
+      </c>
+      <c r="N33" s="85">
+        <f t="shared" si="8"/>
+        <v>5300</v>
+      </c>
+      <c r="O33" s="86">
+        <f t="shared" si="8"/>
+        <v>5300</v>
+      </c>
+      <c r="P33" s="62"/>
+      <c r="Q33" s="63"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="96"/>
+      <c r="B34" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <f>SUM(D34:I34)</f>
+        <v>150</v>
+      </c>
+      <c r="D34" s="69">
+        <v>25</v>
+      </c>
+      <c r="E34" s="70">
+        <v>25</v>
+      </c>
+      <c r="F34" s="70">
+        <v>25</v>
+      </c>
+      <c r="G34" s="70">
+        <v>25</v>
+      </c>
+      <c r="H34" s="70">
+        <v>25</v>
+      </c>
+      <c r="I34" s="71">
+        <v>25</v>
+      </c>
+      <c r="J34" s="81">
+        <f>D34*$P34</f>
+        <v>2500</v>
+      </c>
+      <c r="K34" s="82">
+        <f t="shared" ref="K34:O35" si="9">E34*$P34</f>
+        <v>2500</v>
+      </c>
+      <c r="L34" s="82">
+        <f t="shared" si="9"/>
+        <v>2500</v>
+      </c>
+      <c r="M34" s="82">
+        <f t="shared" si="9"/>
+        <v>2500</v>
+      </c>
+      <c r="N34" s="82">
+        <f t="shared" si="9"/>
+        <v>2500</v>
+      </c>
+      <c r="O34" s="83">
+        <f t="shared" si="9"/>
+        <v>2500</v>
+      </c>
+      <c r="P34" s="62">
+        <v>100</v>
+      </c>
+      <c r="Q34" s="92">
+        <f>SUM(J34:O34)</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" s="96"/>
+      <c r="B35" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <f>SUM(D35:I35)</f>
+        <v>240</v>
+      </c>
+      <c r="D35" s="69">
+        <v>40</v>
+      </c>
+      <c r="E35" s="70">
+        <v>40</v>
+      </c>
+      <c r="F35" s="70">
+        <v>40</v>
+      </c>
+      <c r="G35" s="70">
+        <v>40</v>
+      </c>
+      <c r="H35" s="70">
+        <v>40</v>
+      </c>
+      <c r="I35" s="71">
+        <v>40</v>
+      </c>
+      <c r="J35" s="81">
+        <f t="shared" ref="J35" si="10">D35*$P35</f>
+        <v>2800</v>
+      </c>
+      <c r="K35" s="82">
+        <f t="shared" si="9"/>
+        <v>2800</v>
+      </c>
+      <c r="L35" s="82">
+        <f t="shared" si="9"/>
+        <v>2800</v>
+      </c>
+      <c r="M35" s="82">
+        <f t="shared" si="9"/>
+        <v>2800</v>
+      </c>
+      <c r="N35" s="82">
+        <f t="shared" si="9"/>
+        <v>2800</v>
+      </c>
+      <c r="O35" s="83">
+        <f t="shared" si="9"/>
+        <v>2800</v>
+      </c>
+      <c r="P35" s="62">
+        <v>70</v>
+      </c>
+      <c r="Q35" s="92">
+        <f>SUM(J35:O35)</f>
+        <v>16800</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="96"/>
+      <c r="B36" s="33"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="82"/>
+      <c r="N36" s="82"/>
+      <c r="O36" s="83"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="92"/>
+    </row>
+    <row r="37" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="96"/>
+      <c r="B37" s="33"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="82"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="83"/>
+      <c r="P37" s="93"/>
+      <c r="Q37" s="92"/>
+    </row>
+    <row r="38" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="60"/>
+      <c r="C38" s="58">
+        <f t="shared" ref="C38:O38" si="11">SUM(C40:C41)</f>
+        <v>150</v>
+      </c>
+      <c r="D38" s="72">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="E38" s="73">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="F38" s="73">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="G38" s="73">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="H38" s="73">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="I38" s="74">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="J38" s="84">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+      <c r="K38" s="85">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+      <c r="L38" s="85">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+      <c r="M38" s="85">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+      <c r="N38" s="85">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+      <c r="O38" s="86">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="92"/>
+    </row>
+    <row r="39" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="33"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="81"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="82"/>
+      <c r="M39" s="82"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="83"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="92"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40" s="96"/>
+      <c r="B40" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40">
+        <f>SUM(D40:I40)</f>
+        <v>150</v>
+      </c>
+      <c r="D40" s="69">
+        <v>25</v>
+      </c>
+      <c r="E40" s="70">
+        <v>25</v>
+      </c>
+      <c r="F40" s="70">
+        <v>25</v>
+      </c>
+      <c r="G40" s="70">
+        <v>25</v>
+      </c>
+      <c r="H40" s="70">
+        <v>25</v>
+      </c>
+      <c r="I40" s="71">
+        <v>25</v>
+      </c>
+      <c r="J40" s="81">
+        <f>D40*$P40</f>
+        <v>2000</v>
+      </c>
+      <c r="K40" s="82">
+        <f t="shared" ref="K40:O40" si="12">E40*$P40</f>
+        <v>2000</v>
+      </c>
+      <c r="L40" s="82">
+        <f t="shared" si="12"/>
+        <v>2000</v>
+      </c>
+      <c r="M40" s="82">
+        <f t="shared" si="12"/>
+        <v>2000</v>
+      </c>
+      <c r="N40" s="82">
+        <f t="shared" si="12"/>
+        <v>2000</v>
+      </c>
+      <c r="O40" s="83">
+        <f t="shared" si="12"/>
+        <v>2000</v>
+      </c>
+      <c r="P40" s="62">
+        <v>80</v>
+      </c>
+      <c r="Q40" s="92">
+        <f>SUM(J40:O40)</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="96"/>
+      <c r="B41" s="33"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="82"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="82"/>
+      <c r="N41" s="82"/>
+      <c r="O41" s="83"/>
+      <c r="P41" s="62"/>
+      <c r="Q41" s="92"/>
+    </row>
+    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="60"/>
+      <c r="C42" s="58">
+        <f>SUM(C43:C45)</f>
+        <v>60</v>
+      </c>
+      <c r="D42" s="72">
+        <f t="shared" ref="D42:O42" si="13">SUM(D43:D45)</f>
+        <v>20</v>
+      </c>
+      <c r="E42" s="73">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="F42" s="73">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="G42" s="73">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="73">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="74">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="84">
+        <f t="shared" si="13"/>
+        <v>1000</v>
+      </c>
+      <c r="K42" s="85">
+        <f t="shared" si="13"/>
+        <v>1000</v>
+      </c>
+      <c r="L42" s="85">
+        <f t="shared" si="13"/>
+        <v>1000</v>
+      </c>
+      <c r="M42" s="85">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="N42" s="85">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O42" s="86">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="92"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" s="96"/>
+      <c r="B43" s="32"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="70"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="81"/>
+      <c r="K43" s="82"/>
+      <c r="L43" s="82"/>
+      <c r="M43" s="82"/>
+      <c r="N43" s="82"/>
+      <c r="O43" s="83"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="92"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" s="96"/>
+      <c r="B44" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <f>SUM(D44:I44)</f>
+        <v>60</v>
+      </c>
+      <c r="D44" s="69">
+        <v>20</v>
+      </c>
+      <c r="E44" s="70">
+        <v>20</v>
+      </c>
+      <c r="F44" s="70">
+        <v>20</v>
+      </c>
+      <c r="G44" s="70">
+        <v>0</v>
+      </c>
+      <c r="H44" s="70">
+        <v>0</v>
+      </c>
+      <c r="I44" s="71">
+        <v>0</v>
+      </c>
+      <c r="J44" s="81">
+        <f>D44*$P44</f>
+        <v>1000</v>
+      </c>
+      <c r="K44" s="82">
+        <f t="shared" ref="K44:O44" si="14">E44*$P44</f>
+        <v>1000</v>
+      </c>
+      <c r="L44" s="82">
+        <f t="shared" si="14"/>
+        <v>1000</v>
+      </c>
+      <c r="M44" s="82">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="82">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="O44" s="83">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="62">
+        <v>50</v>
+      </c>
+      <c r="Q44" s="92">
+        <f>SUM(J44:O44)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="96"/>
+      <c r="B45" s="34"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="71"/>
+      <c r="J45" s="81"/>
+      <c r="K45" s="82"/>
+      <c r="L45" s="82"/>
+      <c r="M45" s="82"/>
+      <c r="N45" s="82"/>
+      <c r="O45" s="83"/>
+      <c r="P45" s="62"/>
+      <c r="Q45" s="92"/>
+    </row>
+    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="60"/>
+      <c r="C46" s="58">
+        <f t="shared" ref="C46:O46" si="15">SUM(C48:C50)</f>
+        <v>180</v>
+      </c>
+      <c r="D46" s="72">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="E46" s="73">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="F46" s="73">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="G46" s="73">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="H46" s="73">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="I46" s="74">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="J46" s="84">
+        <f t="shared" si="15"/>
+        <v>1500</v>
+      </c>
+      <c r="K46" s="85">
+        <f t="shared" si="15"/>
+        <v>1500</v>
+      </c>
+      <c r="L46" s="85">
+        <f t="shared" si="15"/>
+        <v>1500</v>
+      </c>
+      <c r="M46" s="85">
+        <f t="shared" si="15"/>
+        <v>1500</v>
+      </c>
+      <c r="N46" s="85">
+        <f t="shared" si="15"/>
+        <v>1500</v>
+      </c>
+      <c r="O46" s="86">
+        <f t="shared" si="15"/>
+        <v>1500</v>
+      </c>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="92"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="33"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="81"/>
+      <c r="K47" s="82"/>
+      <c r="L47" s="82"/>
+      <c r="M47" s="82"/>
+      <c r="N47" s="82"/>
+      <c r="O47" s="83"/>
+      <c r="P47" s="62"/>
+      <c r="Q47" s="92"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" s="96"/>
+      <c r="B48" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48">
+        <f>SUM(D48:I48)</f>
+        <v>60</v>
+      </c>
+      <c r="D48" s="69">
+        <v>10</v>
+      </c>
+      <c r="E48" s="70">
+        <v>10</v>
+      </c>
+      <c r="F48" s="70">
+        <v>10</v>
+      </c>
+      <c r="G48" s="70">
+        <v>10</v>
+      </c>
+      <c r="H48" s="70">
+        <v>10</v>
+      </c>
+      <c r="I48" s="71">
+        <v>10</v>
+      </c>
+      <c r="J48" s="81">
+        <f t="shared" ref="J48:O50" si="16">D48*$P48</f>
+        <v>500</v>
+      </c>
+      <c r="K48" s="82">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="L48" s="82">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="M48" s="82">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="N48" s="82">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="O48" s="83">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="P48" s="62">
+        <v>50</v>
+      </c>
+      <c r="Q48" s="92">
+        <f>SUM(J48:O48)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49" s="33"/>
+      <c r="B49" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49">
+        <f>SUM(D49:I49)</f>
+        <v>60</v>
+      </c>
+      <c r="D49" s="69">
+        <v>10</v>
+      </c>
+      <c r="E49" s="70">
+        <v>10</v>
+      </c>
+      <c r="F49" s="70">
+        <v>10</v>
+      </c>
+      <c r="G49" s="70">
+        <v>10</v>
+      </c>
+      <c r="H49" s="70">
+        <v>10</v>
+      </c>
+      <c r="I49" s="71">
+        <v>10</v>
+      </c>
+      <c r="J49" s="81">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="K49" s="82">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="L49" s="82">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="M49" s="82">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="N49" s="82">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="O49" s="83">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="P49" s="62">
+        <v>50</v>
+      </c>
+      <c r="Q49" s="92">
+        <f>SUM(J49:O49)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="34"/>
+      <c r="B50" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="65">
+        <f>SUM(D50:I50)</f>
+        <v>60</v>
+      </c>
+      <c r="D50" s="75">
+        <v>10</v>
+      </c>
+      <c r="E50" s="76">
+        <v>10</v>
+      </c>
+      <c r="F50" s="76">
+        <v>10</v>
+      </c>
+      <c r="G50" s="76">
+        <v>10</v>
+      </c>
+      <c r="H50" s="76">
+        <v>10</v>
+      </c>
+      <c r="I50" s="77">
+        <v>10</v>
+      </c>
+      <c r="J50" s="87">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="K50" s="88">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="L50" s="88">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="M50" s="88">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="N50" s="88">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="O50" s="89">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="P50" s="64">
+        <v>50</v>
+      </c>
+      <c r="Q50" s="61">
+        <f>SUM(J50:O50)</f>
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D30:I30"/>
+    <mergeCell ref="J30:O30"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16060D28-BA6C-4ED4-9F35-ABFAA3B8932C}">
+  <dimension ref="A1:Q46"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="15" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="4" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="123" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="35">
+        <f>SUM(D4:I4)</f>
+        <v>31800</v>
+      </c>
+      <c r="D4" s="42">
+        <f t="shared" ref="D4:I4" si="0">SUM(J30:J31)</f>
+        <v>5300</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+      <c r="I4" s="43">
+        <f t="shared" si="0"/>
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="124"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="41"/>
+    </row>
+    <row r="6" spans="1:9" ht="34.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="130" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="122" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="35">
+        <f>SUM(D6:I6)</f>
+        <v>4800</v>
+      </c>
+      <c r="D6" s="44">
+        <f>J36</f>
+        <v>800</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" ref="E6:I6" si="1">K36</f>
+        <v>800</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="H6" s="12">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="I6" s="45">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="132" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="35">
+        <f>SUM(D7:I7)</f>
+        <v>3000</v>
+      </c>
+      <c r="D7" s="46">
+        <f>J38</f>
+        <v>1000</v>
+      </c>
+      <c r="E7" s="15">
+        <f>K38</f>
+        <v>1000</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" ref="F7:I7" si="2">L38</f>
+        <v>1000</v>
+      </c>
+      <c r="G7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="47">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="126"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="41"/>
+    </row>
+    <row r="9" spans="1:9" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A9" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="123" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="35">
+        <f>SUM(D9:I9)</f>
+        <v>3000</v>
+      </c>
+      <c r="D9" s="42">
+        <f>SUM(J44:J46)</f>
+        <v>500</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" ref="E9:I9" si="3">SUM(K44:K46)</f>
+        <v>500</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="I9" s="43">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="126"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="41"/>
+    </row>
+    <row r="11" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="123" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="35">
+        <f>SUM(D11:I11)</f>
+        <v>2000</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>500</v>
+      </c>
+      <c r="G11" s="10">
+        <v>500</v>
+      </c>
+      <c r="H11" s="10">
+        <v>500</v>
+      </c>
+      <c r="I11" s="48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="127"/>
+      <c r="B12" s="126"/>
       <c r="C12" s="36"/>
       <c r="D12" s="40"/>
       <c r="E12" s="6"/>
@@ -1907,11 +3449,11 @@
       <c r="H12" s="6"/>
       <c r="I12" s="41"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="124" t="s">
+      <c r="B13" s="123" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="35">
@@ -1937,11 +3479,11 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="127"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="36"/>
       <c r="D14" s="40"/>
       <c r="E14" s="6"/>
@@ -1950,11 +3492,11 @@
       <c r="H14" s="6"/>
       <c r="I14" s="41"/>
     </row>
-    <row r="15" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="131" t="s">
+    <row r="15" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="123" t="s">
+      <c r="B15" s="122" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="35">
@@ -1980,11 +3522,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="128"/>
+      <c r="B16" s="127"/>
       <c r="C16" s="35">
         <f>SUM(D16:I16)</f>
         <v>3000</v>
@@ -2008,11 +3550,11 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="127"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="36"/>
       <c r="D17" s="40"/>
       <c r="E17" s="6"/>
@@ -2021,11 +3563,11 @@
       <c r="H17" s="6"/>
       <c r="I17" s="41"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="123" t="s">
+      <c r="B18" s="122" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="35">
@@ -2051,11 +3593,11 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="130" t="s">
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="129"/>
+      <c r="B19" s="128"/>
       <c r="C19" s="35">
         <f>SUM(D19:I19)</f>
         <v>2400</v>
@@ -2079,7 +3621,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
@@ -2107,7 +3649,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>26</v>
       </c>
@@ -2141,31 +3683,31 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <f>C21-SUM(D21:I21)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="122" t="s">
+    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="122" t="s">
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="136"/>
+      <c r="J26" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="122"/>
-      <c r="L26" s="122"/>
-      <c r="M26" s="122"/>
-      <c r="N26" s="122"/>
-      <c r="O26" s="122"/>
-    </row>
-    <row r="27" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K26" s="136"/>
+      <c r="L26" s="136"/>
+      <c r="M26" s="136"/>
+      <c r="N26" s="136"/>
+      <c r="O26" s="136"/>
+    </row>
+    <row r="27" spans="1:17" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="32"/>
       <c r="B27" s="58" t="s">
         <v>37</v>
@@ -2216,7 +3758,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="94" t="s">
         <v>8</v>
       </c>
@@ -2236,7 +3778,7 @@
       <c r="P28" s="62"/>
       <c r="Q28" s="63"/>
     </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="95" t="s">
         <v>9</v>
       </c>
@@ -2296,7 +3838,7 @@
       <c r="P29" s="62"/>
       <c r="Q29" s="63"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="96"/>
       <c r="B30" s="33" t="s">
         <v>35</v>
@@ -2355,7 +3897,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="96"/>
       <c r="B31" s="33" t="s">
         <v>36</v>
@@ -2414,7 +3956,7 @@
         <v>16800</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="96"/>
       <c r="B32" s="33"/>
       <c r="D32" s="69"/>
@@ -2432,7 +3974,7 @@
       <c r="P32" s="62"/>
       <c r="Q32" s="92"/>
     </row>
-    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="96"/>
       <c r="B33" s="33"/>
       <c r="D33" s="69"/>
@@ -2450,7 +3992,7 @@
       <c r="P33" s="93"/>
       <c r="Q33" s="92"/>
     </row>
-    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="97" t="s">
         <v>10</v>
       </c>
@@ -2510,7 +4052,7 @@
       <c r="P34" s="62"/>
       <c r="Q34" s="92"/>
     </row>
-    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="98" t="s">
         <v>11</v>
       </c>
@@ -2530,7 +4072,7 @@
       <c r="P35" s="62"/>
       <c r="Q35" s="92"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="96"/>
       <c r="B36" s="33" t="s">
         <v>42</v>
@@ -2589,7 +4131,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="96"/>
       <c r="B37" s="33"/>
       <c r="D37" s="69"/>
@@ -2607,7 +4149,7 @@
       <c r="P37" s="62"/>
       <c r="Q37" s="92"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="95" t="s">
         <v>12</v>
       </c>
@@ -2667,7 +4209,7 @@
       <c r="P38" s="62"/>
       <c r="Q38" s="92"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="96"/>
       <c r="B39" s="32"/>
       <c r="D39" s="69"/>
@@ -2685,7 +4227,7 @@
       <c r="P39" s="62"/>
       <c r="Q39" s="92"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="96"/>
       <c r="B40" s="33" t="s">
         <v>43</v>
@@ -2744,7 +4286,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="96"/>
       <c r="B41" s="34"/>
       <c r="D41" s="69"/>
@@ -2762,7 +4304,7 @@
       <c r="P41" s="62"/>
       <c r="Q41" s="92"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="97" t="s">
         <v>13</v>
       </c>
@@ -2822,7 +4364,7 @@
       <c r="P42" s="62"/>
       <c r="Q42" s="92"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="99" t="s">
         <v>14</v>
       </c>
@@ -2842,7 +4384,7 @@
       <c r="P43" s="62"/>
       <c r="Q43" s="92"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="96"/>
       <c r="B44" s="33" t="s">
         <v>44</v>
@@ -2901,7 +4443,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="33"/>
       <c r="B45" s="33" t="s">
         <v>45</v>
@@ -2960,7 +4502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34"/>
       <c r="B46" s="34" t="s">
         <v>46</v>
@@ -3029,33 +4571,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDC5371-1000-4D78-AB43-43C781A04A11}">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A23" sqref="A23"/>
       <selection pane="topRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
-    <col min="23" max="23" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="15" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" customWidth="1"/>
+    <col min="23" max="23" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3084,7 +4626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -3097,7 +4639,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="41"/>
     </row>
-    <row r="4" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -3133,7 +4675,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -3146,8 +4688,8 @@
       <c r="H5" s="6"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:9" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="131" t="s">
+    <row r="6" spans="1:9" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="130" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -3182,8 +4724,8 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="133" t="s">
+    <row r="7" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="132" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="27" t="s">
@@ -3218,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -3231,8 +4773,8 @@
       <c r="H8" s="6"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="134" t="s">
+    <row r="9" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="133" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="24" t="s">
@@ -3267,7 +4809,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -3280,7 +4822,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -3310,7 +4852,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -3323,7 +4865,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="41"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -3353,7 +4895,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -3366,8 +4908,8 @@
       <c r="H14" s="6"/>
       <c r="I14" s="41"/>
     </row>
-    <row r="15" spans="1:9" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="135" t="s">
+    <row r="15" spans="1:9" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="134" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="26" t="s">
@@ -3396,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -3424,7 +4966,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3437,7 +4979,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="41"/>
     </row>
-    <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
@@ -3467,8 +5009,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="136" t="s">
+    <row r="19" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="135" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="30"/>
@@ -3495,7 +5037,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
@@ -3523,7 +5065,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>26</v>
       </c>
@@ -3557,31 +5099,31 @@
         <v>8850</v>
       </c>
     </row>
-    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <f>C21-SUM(D21:I21)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="122" t="s">
+    <row r="26" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="122" t="s">
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="136"/>
+      <c r="J26" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="122"/>
-      <c r="L26" s="122"/>
-      <c r="M26" s="122"/>
-      <c r="N26" s="122"/>
-      <c r="O26" s="122"/>
-    </row>
-    <row r="27" spans="1:28" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K26" s="136"/>
+      <c r="L26" s="136"/>
+      <c r="M26" s="136"/>
+      <c r="N26" s="136"/>
+      <c r="O26" s="136"/>
+    </row>
+    <row r="27" spans="1:28" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="32"/>
       <c r="B27" s="58" t="s">
         <v>37</v>
@@ -3650,7 +5192,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="94" t="s">
         <v>8</v>
       </c>
@@ -3675,7 +5217,7 @@
       <c r="AA28" s="104"/>
       <c r="AB28" s="105"/>
     </row>
-    <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="95" t="s">
         <v>9</v>
       </c>
@@ -3740,7 +5282,7 @@
       <c r="AA29" s="104"/>
       <c r="AB29" s="105"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" s="96"/>
       <c r="B30" s="33" t="s">
         <v>35</v>
@@ -3817,7 +5359,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="96"/>
       <c r="B31" s="33" t="s">
         <v>36</v>
@@ -3894,7 +5436,7 @@
         <v>16800</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="96"/>
       <c r="B32" s="33"/>
       <c r="D32" s="69"/>
@@ -3917,7 +5459,7 @@
       <c r="AA32" s="104"/>
       <c r="AB32" s="105"/>
     </row>
-    <row r="33" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="96"/>
       <c r="B33" s="33"/>
       <c r="D33" s="69"/>
@@ -3940,7 +5482,7 @@
       <c r="AA33" s="104"/>
       <c r="AB33" s="105"/>
     </row>
-    <row r="34" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="97" t="s">
         <v>10</v>
       </c>
@@ -4005,7 +5547,7 @@
       <c r="AA34" s="104"/>
       <c r="AB34" s="105"/>
     </row>
-    <row r="35" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="98" t="s">
         <v>11</v>
       </c>
@@ -4030,7 +5572,7 @@
       <c r="AA35" s="104"/>
       <c r="AB35" s="105"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" s="96"/>
       <c r="B36" s="33" t="s">
         <v>42</v>
@@ -4107,7 +5649,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="96"/>
       <c r="B37" s="33"/>
       <c r="D37" s="69"/>
@@ -4130,7 +5672,7 @@
       <c r="AA37" s="104"/>
       <c r="AB37" s="105"/>
     </row>
-    <row r="38" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="95" t="s">
         <v>12</v>
       </c>
@@ -4195,7 +5737,7 @@
       <c r="AA38" s="104"/>
       <c r="AB38" s="105"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" s="96"/>
       <c r="B39" s="32"/>
       <c r="D39" s="69"/>
@@ -4218,7 +5760,7 @@
       <c r="AA39" s="104"/>
       <c r="AB39" s="105"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="96"/>
       <c r="B40" s="33" t="s">
         <v>43</v>
@@ -4295,7 +5837,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="96"/>
       <c r="B41" s="34"/>
       <c r="D41" s="69"/>
@@ -4318,7 +5860,7 @@
       <c r="AA41" s="104"/>
       <c r="AB41" s="105"/>
     </row>
-    <row r="42" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="97" t="s">
         <v>13</v>
       </c>
@@ -4383,7 +5925,7 @@
       <c r="AA42" s="104"/>
       <c r="AB42" s="105"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" s="99" t="s">
         <v>14</v>
       </c>
@@ -4408,7 +5950,7 @@
       <c r="AA43" s="104"/>
       <c r="AB43" s="105"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" s="96"/>
       <c r="B44" s="33" t="s">
         <v>44</v>
@@ -4485,7 +6027,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="33"/>
       <c r="B45" s="33" t="s">
         <v>45</v>
@@ -4562,7 +6104,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34"/>
       <c r="B46" s="34" t="s">
         <v>46</v>
@@ -4639,8 +6181,8 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="W48" s="100" t="s">
         <v>49</v>
       </c>
@@ -4664,11 +6206,11 @@
         <v>55800</v>
       </c>
     </row>
-    <row r="49" spans="23:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="23:28" x14ac:dyDescent="0.3">
       <c r="W49" s="62"/>
       <c r="AB49" s="63"/>
     </row>
-    <row r="50" spans="23:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="23:28" x14ac:dyDescent="0.3">
       <c r="W50" s="62" t="s">
         <v>50</v>
       </c>
@@ -4692,11 +6234,11 @@
         <v>17700</v>
       </c>
     </row>
-    <row r="51" spans="23:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="23:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="W51" s="62"/>
       <c r="AB51" s="63"/>
     </row>
-    <row r="52" spans="23:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="23:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="W52" s="58" t="s">
         <v>47</v>
       </c>
@@ -4712,7 +6254,7 @@
         <v>73500</v>
       </c>
     </row>
-    <row r="55" spans="23:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="23:28" x14ac:dyDescent="0.3">
       <c r="Z55" s="118">
         <f>(Z50/Z52)*100</f>
         <v>34.705882352941174</v>
@@ -4732,26 +6274,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I21"/>
+    <sheetView zoomScale="76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="15" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:9" ht="33.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4780,7 +6322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -4793,7 +6335,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="41"/>
     </row>
-    <row r="4" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -4829,7 +6371,7 @@
         <v>5300</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -4842,7 +6384,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:9" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
@@ -4878,7 +6420,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
@@ -4914,7 +6456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -4927,7 +6469,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -4963,7 +6505,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -4976,7 +6518,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -5006,7 +6548,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -5019,7 +6561,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="41"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -5049,7 +6591,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -5062,7 +6604,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="41"/>
     </row>
-    <row r="15" spans="1:9" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>20</v>
       </c>
@@ -5092,7 +6634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
@@ -5120,7 +6662,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -5133,7 +6675,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="41"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
@@ -5163,7 +6705,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>24</v>
       </c>
@@ -5191,7 +6733,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>25</v>
       </c>
@@ -5219,7 +6761,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>26</v>
       </c>
@@ -5253,31 +6795,31 @@
         <v>12400</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <f>C21-SUM(D21:I21)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="122" t="s">
+    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="122"/>
-      <c r="H26" s="122"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="122" t="s">
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="136"/>
+      <c r="J26" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="122"/>
-      <c r="L26" s="122"/>
-      <c r="M26" s="122"/>
-      <c r="N26" s="122"/>
-      <c r="O26" s="122"/>
-    </row>
-    <row r="27" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K26" s="136"/>
+      <c r="L26" s="136"/>
+      <c r="M26" s="136"/>
+      <c r="N26" s="136"/>
+      <c r="O26" s="136"/>
+    </row>
+    <row r="27" spans="1:17" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="32"/>
       <c r="B27" s="58" t="s">
         <v>37</v>
@@ -5328,7 +6870,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="94" t="s">
         <v>8</v>
       </c>
@@ -5348,7 +6890,7 @@
       <c r="P28" s="62"/>
       <c r="Q28" s="63"/>
     </row>
-    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="95" t="s">
         <v>9</v>
       </c>
@@ -5408,7 +6950,7 @@
       <c r="P29" s="62"/>
       <c r="Q29" s="63"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="96"/>
       <c r="B30" s="33" t="s">
         <v>35</v>
@@ -5467,7 +7009,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="96"/>
       <c r="B31" s="33" t="s">
         <v>36</v>
@@ -5526,7 +7068,7 @@
         <v>16800</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="96"/>
       <c r="B32" s="33"/>
       <c r="D32" s="69"/>
@@ -5544,7 +7086,7 @@
       <c r="P32" s="62"/>
       <c r="Q32" s="92"/>
     </row>
-    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="96"/>
       <c r="B33" s="33"/>
       <c r="D33" s="69"/>
@@ -5562,7 +7104,7 @@
       <c r="P33" s="93"/>
       <c r="Q33" s="92"/>
     </row>
-    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="97" t="s">
         <v>10</v>
       </c>
@@ -5622,7 +7164,7 @@
       <c r="P34" s="62"/>
       <c r="Q34" s="92"/>
     </row>
-    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="98" t="s">
         <v>11</v>
       </c>
@@ -5642,7 +7184,7 @@
       <c r="P35" s="62"/>
       <c r="Q35" s="92"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="96"/>
       <c r="B36" s="33" t="s">
         <v>42</v>
@@ -5701,7 +7243,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="96"/>
       <c r="B37" s="33"/>
       <c r="D37" s="69"/>
@@ -5719,7 +7261,7 @@
       <c r="P37" s="62"/>
       <c r="Q37" s="92"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="95" t="s">
         <v>12</v>
       </c>
@@ -5779,7 +7321,7 @@
       <c r="P38" s="62"/>
       <c r="Q38" s="92"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="96"/>
       <c r="B39" s="32"/>
       <c r="D39" s="69"/>
@@ -5797,7 +7339,7 @@
       <c r="P39" s="62"/>
       <c r="Q39" s="92"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="96"/>
       <c r="B40" s="33" t="s">
         <v>43</v>
@@ -5856,7 +7398,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="96"/>
       <c r="B41" s="34"/>
       <c r="D41" s="69"/>
@@ -5874,7 +7416,7 @@
       <c r="P41" s="62"/>
       <c r="Q41" s="92"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="97" t="s">
         <v>13</v>
       </c>
@@ -5934,7 +7476,7 @@
       <c r="P42" s="62"/>
       <c r="Q42" s="92"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="99" t="s">
         <v>14</v>
       </c>
@@ -5954,7 +7496,7 @@
       <c r="P43" s="62"/>
       <c r="Q43" s="92"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="96"/>
       <c r="B44" s="33" t="s">
         <v>44</v>
@@ -6013,7 +7555,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="33"/>
       <c r="B45" s="33" t="s">
         <v>45</v>
@@ -6072,7 +7614,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="34"/>
       <c r="B46" s="34" t="s">
         <v>46</v>

</xml_diff>